<commit_message>
updated jax fc code
</commit_message>
<xml_diff>
--- a/Resources/Steps.xlsx
+++ b/Resources/Steps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekeymon\Documents\data-analysis\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDB15FE-40DE-48CE-9982-7D0C10E9D973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35DAD4B-DAD0-482C-AF43-174787B89081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{547509CD-F3D7-4A96-B100-57F3C154F68B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Import libraries</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Add column Org</t>
   </si>
   <si>
-    <t>Delete Comment column</t>
-  </si>
-  <si>
     <t>Check total count against resource file to ensure data is correct</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>Merge FC + SO</t>
+  </si>
+  <si>
+    <t>New data frame with deleted Comment column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort by Date, then Item </t>
   </si>
 </sst>
 </file>
@@ -515,9 +518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DB2C8D-604D-4B90-B5E5-9373F2219062}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -537,22 +542,22 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -563,19 +568,19 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -586,16 +591,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -606,16 +611,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -626,16 +631,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -715,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -723,55 +728,71 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>